<commit_message>
ЧМ Pract 2 excel updated
</commit_message>
<xml_diff>
--- a/Course III/ЧМ/Pract 2/gauss_excel.xlsx
+++ b/Course III/ЧМ/Pract 2/gauss_excel.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Disk II/Projects/KIP/Course III/ЧМ/2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgiydemo/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="1220" windowWidth="10560" windowHeight="13440" tabRatio="500"/>
+    <workbookView xWindow="1660" yWindow="1440" windowWidth="21520" windowHeight="14960" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Вариант 4</t>
   </si>
@@ -45,7 +46,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -84,6 +85,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -147,7 +154,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -160,6 +167,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
@@ -451,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScale="117" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -877,4 +885,430 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="6">
+        <v>0.63</v>
+      </c>
+      <c r="B1" s="10">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C1" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="D1" s="7">
+        <v>0.34</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.71</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.34</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <f>A1</f>
+        <v>0.63</v>
+      </c>
+      <c r="B5" s="8">
+        <f>B1</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C5" s="8">
+        <f>C1</f>
+        <v>0.15</v>
+      </c>
+      <c r="D5" s="9">
+        <f>D1</f>
+        <v>0.34</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="1"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <f t="array" ref="A6:D6">A2:D2-$A$1:$D$1*(A2/$A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="B6" s="8">
+        <v>8.9285714285714288E-2</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.67428571428571427</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.33904761904761904</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <f t="array" ref="A7:D7">A3:D3-$A$1:$D$1*(A3/$A$1)</f>
+        <v>0</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.33785714285714286</v>
+      </c>
+      <c r="C7" s="8">
+        <v>9.285714285714286E-2</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.30380952380952381</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <f t="shared" ref="A9:D10" si="0">A5</f>
+        <v>0.63</v>
+      </c>
+      <c r="B9" s="8">
+        <f t="shared" si="0"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B10" s="8">
+        <f t="shared" si="0"/>
+        <v>8.9285714285714288E-2</v>
+      </c>
+      <c r="C10" s="8">
+        <f t="shared" si="0"/>
+        <v>0.67428571428571427</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>0.33904761904761904</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <f t="array" ref="A11:D11">A7:D7-$A$6:$D$6*(B7/$B$6)</f>
+        <v>0</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8">
+        <v>-2.4586399999999995</v>
+      </c>
+      <c r="D11" s="9">
+        <v>-0.97914666666666661</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <f t="array" ref="A14:D14">(A9:D9-A16:D16*C9-A15:D15*B9)/A9</f>
+        <v>1</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.38844962165171715</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <f t="array" ref="F14:F16">MMULT(MINVERSE(A1:C3),D1:D3)</f>
+        <v>0.3884496216517172</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <f t="array" ref="A15:D15">(A10:D10-A16:D16*C10)/B10</f>
+        <v>0</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.78976995412097728</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1">
+        <v>0.7897699541209775</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <f t="array" ref="A16:D16">A11:D11/C11</f>
+        <v>0</v>
+      </c>
+      <c r="B16" s="8">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.39824726949316158</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>0.39824726949316158</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>